<commit_message>
update main.py + decks + 다시 공부하기 기능
</commit_message>
<xml_diff>
--- a/decks/N4 동작 테스트용.xlsx
+++ b/decks/N4 동작 테스트용.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -62,90 +62,6 @@
   </si>
   <si>
     <t>デパートで買(か)い物(もの)をします。/백화점에서 쇼핑합니다。</t>
-  </si>
-  <si>
-    <t>スーパー</t>
-  </si>
-  <si>
-    <t>すーぱー</t>
-  </si>
-  <si>
-    <t>슈퍼마켓</t>
-  </si>
-  <si>
-    <t>スーパーで野菜(やさい)を買(か)います。/슈퍼에서 채소를 삽니다。</t>
-  </si>
-  <si>
-    <t>コンビニ</t>
-  </si>
-  <si>
-    <t>こんびに</t>
-  </si>
-  <si>
-    <t>편의점</t>
-  </si>
-  <si>
-    <t>コンビニで飲(の)み物(もの)を買(か)います。/편의점에서 음료를 삽니다。</t>
-  </si>
-  <si>
-    <t>アパート</t>
-  </si>
-  <si>
-    <t>あぱーと</t>
-  </si>
-  <si>
-    <t>아파트</t>
-  </si>
-  <si>
-    <t>アパートに住(す)んでいます。/아파트에 살고 있습니다。</t>
-  </si>
-  <si>
-    <t>マンション</t>
-  </si>
-  <si>
-    <t>まんしょん</t>
-  </si>
-  <si>
-    <t>맨션형 아파트</t>
-  </si>
-  <si>
-    <t>マンションに住(す)んでいます。/맨션에 살고 있습니다。</t>
-  </si>
-  <si>
-    <t>エレベーター</t>
-  </si>
-  <si>
-    <t>えれべーたー</t>
-  </si>
-  <si>
-    <t>엘리베이터</t>
-  </si>
-  <si>
-    <t>エレベーターを使(つか)います。/엘리베이터를 사용합니다。</t>
-  </si>
-  <si>
-    <t>エスカレーター</t>
-  </si>
-  <si>
-    <t>えすかれーたー</t>
-  </si>
-  <si>
-    <t>에스컬레이터</t>
-  </si>
-  <si>
-    <t>エスカレーターで上(あ)がります。/에스컬레이터로 올라갑니다。</t>
-  </si>
-  <si>
-    <t>タクシー</t>
-  </si>
-  <si>
-    <t>たくしー</t>
-  </si>
-  <si>
-    <t>택시</t>
-  </si>
-  <si>
-    <t>タクシーに乗(の)ります。/택시를 탑니다。</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1515,156 +1431,23 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" ht="42.15" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" t="s" s="12">
         <v>14</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D4" t="s" s="12">
         <v>15</v>
       </c>
-      <c r="E4" t="s" s="8">
+      <c r="E4" t="s" s="13">
         <v>16</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s" s="8">
-        <v>24</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="8">
-        <v>28</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s" s="8">
-        <v>32</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s" s="12">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s" s="12">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s" s="12">
-        <v>43</v>
-      </c>
-      <c r="E11" t="s" s="13">
-        <v>44</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>